<commit_message>
microcode add, addi, nand, lw, sw
</commit_message>
<xml_diff>
--- a/microcode.xlsx
+++ b/microcode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vivek\room\courses\systems\project1\project-files\student\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dchang0524/Desktop/GT/CS2200/CS2200_Project_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174B55FD-67AC-4347-849B-90D3BF2DDC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6D62DA-9171-DF4C-AA7C-BFA9FCCAAB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3795" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="740" windowWidth="24960" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Index</t>
   </si>
@@ -205,12 +205,114 @@
   <si>
     <t>CmpTargetHi</t>
   </si>
+  <si>
+    <t>FETCH1</t>
+  </si>
+  <si>
+    <t>A &lt;- PC</t>
+  </si>
+  <si>
+    <t>PC &lt;- PC + 1</t>
+  </si>
+  <si>
+    <t>FETCH2</t>
+  </si>
+  <si>
+    <t>MAR &lt;- PC</t>
+  </si>
+  <si>
+    <t>FETCH3</t>
+  </si>
+  <si>
+    <t>IR &lt;- MEM[PC_prev]</t>
+  </si>
+  <si>
+    <t>DECODE</t>
+  </si>
+  <si>
+    <t>Check IR for next state</t>
+  </si>
+  <si>
+    <t>ADD1</t>
+  </si>
+  <si>
+    <t>ADD3</t>
+  </si>
+  <si>
+    <t>ADD2</t>
+  </si>
+  <si>
+    <t>B &lt;- Reg(IR[3:0])</t>
+  </si>
+  <si>
+    <t>A &lt;- Reg(IR[23:20])</t>
+  </si>
+  <si>
+    <t>Reg(IR[27:24]) &lt;- A + B</t>
+  </si>
+  <si>
+    <t>NAND1</t>
+  </si>
+  <si>
+    <t>NAND2</t>
+  </si>
+  <si>
+    <t>NAND3</t>
+  </si>
+  <si>
+    <t>Reg(IR[27:24]) &lt;- NAND(A, B)</t>
+  </si>
+  <si>
+    <t>ADDI1</t>
+  </si>
+  <si>
+    <t>B &lt;- SEXT(SEXT[19:0])</t>
+  </si>
+  <si>
+    <t>ADDI2</t>
+  </si>
+  <si>
+    <t>ADDI3</t>
+  </si>
+  <si>
+    <t>LW1</t>
+  </si>
+  <si>
+    <t>LW2</t>
+  </si>
+  <si>
+    <t>LW3</t>
+  </si>
+  <si>
+    <t>MAR &lt;- A + B</t>
+  </si>
+  <si>
+    <t>DR = MEM[A+B]</t>
+  </si>
+  <si>
+    <t>MEM[A+B] &lt;- SR</t>
+  </si>
+  <si>
+    <t>LW4</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -485,6 +587,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,36 +849,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W73" sqref="W73"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="14.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="2.69921875" customWidth="1"/>
-    <col min="8" max="8" width="2.296875" customWidth="1"/>
-    <col min="9" max="9" width="9.19921875" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
     <col min="10" max="28" width="9.5" customWidth="1"/>
-    <col min="29" max="29" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9.5" customWidth="1"/>
-    <col min="32" max="32" width="4.69921875" customWidth="1"/>
-    <col min="33" max="33" width="11.69921875" customWidth="1"/>
-    <col min="34" max="34" width="27.69921875" customWidth="1"/>
-    <col min="35" max="35" width="10.19921875" customWidth="1"/>
-    <col min="36" max="38" width="7.69921875" customWidth="1"/>
-    <col min="39" max="39" width="13.19921875" customWidth="1"/>
-    <col min="40" max="40" width="15.19921875" customWidth="1"/>
-    <col min="41" max="41" width="7.69921875" customWidth="1"/>
-    <col min="42" max="42" width="10.69921875" customWidth="1"/>
-    <col min="43" max="43" width="7.69921875" customWidth="1"/>
-    <col min="44" max="1028" width="12.69921875" customWidth="1"/>
+    <col min="32" max="32" width="4.6640625" customWidth="1"/>
+    <col min="33" max="33" width="11.6640625" customWidth="1"/>
+    <col min="34" max="34" width="27.6640625" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" customWidth="1"/>
+    <col min="36" max="38" width="7.6640625" customWidth="1"/>
+    <col min="39" max="39" width="13.1640625" customWidth="1"/>
+    <col min="40" max="40" width="15.1640625" customWidth="1"/>
+    <col min="41" max="41" width="7.6640625" customWidth="1"/>
+    <col min="42" max="42" width="10.6640625" customWidth="1"/>
+    <col min="43" max="43" width="7.6640625" customWidth="1"/>
+    <col min="44" max="1028" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="30.75" customHeight="1">
+    <row r="1" spans="1:43" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,11 +979,13 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:43" ht="14.25" customHeight="1">
+    <row r="2" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C2" s="14">
         <v>0</v>
       </c>
@@ -897,11 +1002,11 @@
         <v>0</v>
       </c>
       <c r="H2" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="15">
         <f t="shared" ref="I2:I33" si="0">BIN2DEC(_xlfn.CONCAT(C2:H2))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="14">
         <v>0</v>
@@ -928,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="R2" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="14">
         <v>0</v>
@@ -943,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="W2" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="14">
         <v>0</v>
@@ -972,14 +1077,22 @@
       <c r="AF2" s="4"/>
       <c r="AG2" s="6" t="str">
         <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J2, K2, L2, M2),1),     BIN2HEX(_xlfn.CONCAT(N2,O2,P2,Q2),1),     BIN2HEX(_xlfn.CONCAT(R2,S2,T2,U2),1),     BIN2HEX(_xlfn.CONCAT(V2,W2,X2,Y2),1),     BIN2HEX(_xlfn.CONCAT(Z2,AA2,AB2,AC2),1),     BIN2HEX(_xlfn.CONCAT(AD2,AE2,C2,D2),1),     BIN2HEX(_xlfn.CONCAT(E2,F2,G2,H2),1) )</f>
-        <v>0000000</v>
+        <v>00C4001</v>
+      </c>
+      <c r="AJ2" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK2" s="33" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="14.25" customHeight="1">
+    <row r="3" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C3" s="14">
         <v>0</v>
       </c>
@@ -993,14 +1106,14 @@
         <v>0</v>
       </c>
       <c r="G3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="14">
         <v>0</v>
       </c>
       <c r="I3" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" s="14">
         <v>0</v>
@@ -1009,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="14">
         <v>0</v>
@@ -1036,13 +1149,13 @@
         <v>0</v>
       </c>
       <c r="U3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="14">
         <v>0</v>
       </c>
       <c r="W3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="14">
         <v>0</v>
@@ -1071,14 +1184,20 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="6" t="str">
         <f t="shared" ref="AG3:AG65" si="1">_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J3, K3, L3, M3),1),     BIN2HEX(_xlfn.CONCAT(N3,O3,P3,Q3),1),     BIN2HEX(_xlfn.CONCAT(R3,S3,T3,U3),1),     BIN2HEX(_xlfn.CONCAT(V3,W3,X3,Y3),1),     BIN2HEX(_xlfn.CONCAT(Z3,AA3,AB3,AC3),1),     BIN2HEX(_xlfn.CONCAT(AD3,AE3,C3,D3),1),     BIN2HEX(_xlfn.CONCAT(E3,F3,G3,H3),1) )</f>
-        <v>0000000</v>
-      </c>
+        <v>2014002</v>
+      </c>
+      <c r="AJ3" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL3" s="33"/>
     </row>
-    <row r="4" spans="1:43" ht="14.25" customHeight="1">
+    <row r="4" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C4" s="14">
         <v>0</v>
       </c>
@@ -1092,14 +1211,14 @@
         <v>0</v>
       </c>
       <c r="G4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4" s="14">
         <v>0</v>
@@ -1132,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="14">
         <v>0</v>
@@ -1147,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="14">
         <v>0</v>
@@ -1170,15 +1289,20 @@
       <c r="AF4" s="4"/>
       <c r="AG4" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0021003</v>
+      </c>
+      <c r="AJ4" s="33" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="14.25" customHeight="1">
+    <row r="5" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <f t="shared" ref="A5:A33" si="2">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C5" s="14">
         <v>0</v>
       </c>
@@ -1265,20 +1389,25 @@
         <v>0</v>
       </c>
       <c r="AE5" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5" s="4"/>
       <c r="AG5" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0000040</v>
+      </c>
+      <c r="AJ5" s="33" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="14.25" customHeight="1">
+    <row r="6" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C6" s="14">
         <v>0</v>
       </c>
@@ -1289,23 +1418,23 @@
         <v>0</v>
       </c>
       <c r="F6" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="14">
         <v>0</v>
       </c>
       <c r="H6" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J6" s="14">
         <v>0</v>
       </c>
       <c r="K6" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="14">
         <v>0</v>
@@ -1326,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="14">
         <v>0</v>
@@ -1350,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="Z6" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="14">
         <v>0</v>
@@ -1369,16 +1498,21 @@
       </c>
       <c r="AF6" s="4"/>
       <c r="AG6" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J6, K6, L6, M6),1),     BIN2HEX(_xlfn.CONCAT(N6,O6,P6,Q6),1),     BIN2HEX(_xlfn.CONCAT(R6,S6,T6,U6),1),     BIN2HEX(_xlfn.CONCAT(V6,W6,X6,Y6),1),     BIN2HEX(_xlfn.CONCAT(Z6,AA6,AB6,AC6),1),     BIN2HEX(_xlfn.CONCAT(AD6,AE6,C6,D6),1),     BIN2HEX(_xlfn.CONCAT(E6,F6,G6,H6),1) )</f>
-        <v>0000000</v>
+        <f t="shared" ref="AG6:AG18" si="3">_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J6, K6, L6, M6),1),     BIN2HEX(_xlfn.CONCAT(N6,O6,P6,Q6),1),     BIN2HEX(_xlfn.CONCAT(R6,S6,T6,U6),1),     BIN2HEX(_xlfn.CONCAT(V6,W6,X6,Y6),1),     BIN2HEX(_xlfn.CONCAT(Z6,AA6,AB6,AC6),1),     BIN2HEX(_xlfn.CONCAT(AD6,AE6,C6,D6),1),     BIN2HEX(_xlfn.CONCAT(E6,F6,G6,H6),1) )</f>
+        <v>4080805</v>
+      </c>
+      <c r="AJ6" s="33" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:43" ht="14.25" customHeight="1">
+    <row r="7" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="14">
         <v>0</v>
       </c>
@@ -1389,20 +1523,20 @@
         <v>0</v>
       </c>
       <c r="F7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="14">
         <v>0</v>
       </c>
       <c r="I7" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="14">
         <v>0</v>
@@ -1423,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="14">
         <v>0</v>
@@ -1450,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="Z7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7" s="14">
         <v>0</v>
@@ -1469,16 +1603,21 @@
       </c>
       <c r="AF7" s="4"/>
       <c r="AG7" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J7, K7, L7, M7),1),     BIN2HEX(_xlfn.CONCAT(N7,O7,P7,Q7),1),     BIN2HEX(_xlfn.CONCAT(R7,S7,T7,U7),1),     BIN2HEX(_xlfn.CONCAT(V7,W7,X7,Y7),1),     BIN2HEX(_xlfn.CONCAT(Z7,AA7,AB7,AC7),1),     BIN2HEX(_xlfn.CONCAT(AD7,AE7,C7,D7),1),     BIN2HEX(_xlfn.CONCAT(E7,F7,G7,H7),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>8100806</v>
+      </c>
+      <c r="AJ7" s="33" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:43" ht="14.25" customHeight="1">
+    <row r="8" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C8" s="14">
         <v>0</v>
       </c>
@@ -1520,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="14">
         <v>0</v>
@@ -1544,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="14">
         <v>0</v>
@@ -1569,16 +1708,21 @@
       </c>
       <c r="AF8" s="4"/>
       <c r="AG8" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J8, K8, L8, M8),1),     BIN2HEX(_xlfn.CONCAT(N8,O8,P8,Q8),1),     BIN2HEX(_xlfn.CONCAT(R8,S8,T8,U8),1),     BIN2HEX(_xlfn.CONCAT(V8,W8,X8,Y8),1),     BIN2HEX(_xlfn.CONCAT(Z8,AA8,AB8,AC8),1),     BIN2HEX(_xlfn.CONCAT(AD8,AE8,C8,D8),1),     BIN2HEX(_xlfn.CONCAT(E8,F8,G8,H8),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>0202000</v>
+      </c>
+      <c r="AJ8" s="33" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:43" ht="14.25" customHeight="1">
+    <row r="9" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C9" s="14">
         <v>0</v>
       </c>
@@ -1586,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="14">
         <v>0</v>
@@ -1599,13 +1743,13 @@
       </c>
       <c r="I9" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="14">
         <v>0</v>
       </c>
       <c r="K9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="14">
         <v>0</v>
@@ -1626,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="14">
         <v>0</v>
@@ -1650,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="Z9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="14">
         <v>0</v>
@@ -1669,16 +1813,21 @@
       </c>
       <c r="AF9" s="4"/>
       <c r="AG9" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J9, K9, L9, M9),1),     BIN2HEX(_xlfn.CONCAT(N9,O9,P9,Q9),1),     BIN2HEX(_xlfn.CONCAT(R9,S9,T9,U9),1),     BIN2HEX(_xlfn.CONCAT(V9,W9,X9,Y9),1),     BIN2HEX(_xlfn.CONCAT(Z9,AA9,AB9,AC9),1),     BIN2HEX(_xlfn.CONCAT(AD9,AE9,C9,D9),1),     BIN2HEX(_xlfn.CONCAT(E9,F9,G9,H9),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>4080808</v>
+      </c>
+      <c r="AJ9" s="33" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:43" ht="14.25" customHeight="1">
+    <row r="10" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B10" s="14"/>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C10" s="14">
         <v>0</v>
       </c>
@@ -1686,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="14">
         <v>0</v>
@@ -1695,14 +1844,14 @@
         <v>0</v>
       </c>
       <c r="H10" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J10" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="14">
         <v>0</v>
@@ -1723,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="14">
         <v>0</v>
@@ -1769,16 +1918,21 @@
       </c>
       <c r="AF10" s="4"/>
       <c r="AG10" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J10, K10, L10, M10),1),     BIN2HEX(_xlfn.CONCAT(N10,O10,P10,Q10),1),     BIN2HEX(_xlfn.CONCAT(R10,S10,T10,U10),1),     BIN2HEX(_xlfn.CONCAT(V10,W10,X10,Y10),1),     BIN2HEX(_xlfn.CONCAT(Z10,AA10,AB10,AC10),1),     BIN2HEX(_xlfn.CONCAT(AD10,AE10,C10,D10),1),     BIN2HEX(_xlfn.CONCAT(E10,F10,G10,H10),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>8100009</v>
+      </c>
+      <c r="AJ10" s="33" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:43" ht="14.25" customHeight="1">
+    <row r="11" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C11" s="14">
         <v>0</v>
       </c>
@@ -1811,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="14">
         <v>0</v>
@@ -1820,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="14">
         <v>0</v>
@@ -1844,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="14">
         <v>0</v>
@@ -1869,16 +2023,21 @@
       </c>
       <c r="AF11" s="4"/>
       <c r="AG11" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J11, K11, L11, M11),1),     BIN2HEX(_xlfn.CONCAT(N11,O11,P11,Q11),1),     BIN2HEX(_xlfn.CONCAT(R11,S11,T11,U11),1),     BIN2HEX(_xlfn.CONCAT(V11,W11,X11,Y11),1),     BIN2HEX(_xlfn.CONCAT(Z11,AA11,AB11,AC11),1),     BIN2HEX(_xlfn.CONCAT(AD11,AE11,C11,D11),1),     BIN2HEX(_xlfn.CONCAT(E11,F11,G11,H11),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>1202000</v>
+      </c>
+      <c r="AJ11" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:43" ht="14.25" customHeight="1">
+    <row r="12" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="C12" s="14">
         <v>0</v>
       </c>
@@ -1886,26 +2045,26 @@
         <v>0</v>
       </c>
       <c r="E12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="14">
         <v>0</v>
       </c>
       <c r="G12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J12" s="14">
         <v>0</v>
       </c>
       <c r="K12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="14">
         <v>0</v>
@@ -1926,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="14">
         <v>0</v>
@@ -1950,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="Z12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12" s="14">
         <v>0</v>
@@ -1969,16 +2128,22 @@
       </c>
       <c r="AF12" s="4"/>
       <c r="AG12" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J12, K12, L12, M12),1),     BIN2HEX(_xlfn.CONCAT(N12,O12,P12,Q12),1),     BIN2HEX(_xlfn.CONCAT(R12,S12,T12,U12),1),     BIN2HEX(_xlfn.CONCAT(V12,W12,X12,Y12),1),     BIN2HEX(_xlfn.CONCAT(Z12,AA12,AB12,AC12),1),     BIN2HEX(_xlfn.CONCAT(AD12,AE12,C12,D12),1),     BIN2HEX(_xlfn.CONCAT(E12,F12,G12,H12),1) )</f>
-        <v>0000000</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>408080B</v>
+      </c>
+      <c r="AJ12" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM12" s="33"/>
     </row>
-    <row r="13" spans="1:43" ht="14.25" customHeight="1">
+    <row r="13" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="C13" s="14">
         <v>0</v>
       </c>
@@ -1986,10 +2151,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="14">
         <v>0</v>
@@ -1999,10 +2164,10 @@
       </c>
       <c r="I13" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="14">
         <v>0</v>
@@ -2023,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="14">
         <v>0</v>
@@ -2038,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="14">
         <v>0</v>
@@ -2069,16 +2234,21 @@
       </c>
       <c r="AF13" s="4"/>
       <c r="AG13" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J13, K13, L13, M13),1),     BIN2HEX(_xlfn.CONCAT(N13,O13,P13,Q13),1),     BIN2HEX(_xlfn.CONCAT(R13,S13,T13,U13),1),     BIN2HEX(_xlfn.CONCAT(V13,W13,X13,Y13),1),     BIN2HEX(_xlfn.CONCAT(Z13,AA13,AB13,AC13),1),     BIN2HEX(_xlfn.CONCAT(AD13,AE13,C13,D13),1),     BIN2HEX(_xlfn.CONCAT(E13,F13,G13,H13),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>810800C</v>
+      </c>
+      <c r="AJ13" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="14.25" customHeight="1">
+    <row r="14" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="C14" s="14">
         <v>0</v>
       </c>
@@ -2120,7 +2290,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="14">
         <v>0</v>
@@ -2144,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="14">
         <v>0</v>
@@ -2169,16 +2339,21 @@
       </c>
       <c r="AF14" s="4"/>
       <c r="AG14" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J14, K14, L14, M14),1),     BIN2HEX(_xlfn.CONCAT(N14,O14,P14,Q14),1),     BIN2HEX(_xlfn.CONCAT(R14,S14,T14,U14),1),     BIN2HEX(_xlfn.CONCAT(V14,W14,X14,Y14),1),     BIN2HEX(_xlfn.CONCAT(Z14,AA14,AB14,AC14),1),     BIN2HEX(_xlfn.CONCAT(AD14,AE14,C14,D14),1),     BIN2HEX(_xlfn.CONCAT(E14,F14,G14,H14),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>0202000</v>
+      </c>
+      <c r="AJ14" s="33" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:43" ht="14.25" customHeight="1">
+    <row r="15" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C15" s="14">
         <v>0</v>
       </c>
@@ -2186,26 +2361,26 @@
         <v>0</v>
       </c>
       <c r="E15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="14">
         <v>0</v>
       </c>
       <c r="I15" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J15" s="14">
         <v>0</v>
       </c>
       <c r="K15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="14">
         <v>0</v>
@@ -2226,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" s="14">
         <v>0</v>
@@ -2250,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="Z15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15" s="14">
         <v>0</v>
@@ -2269,16 +2444,21 @@
       </c>
       <c r="AF15" s="4"/>
       <c r="AG15" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J15, K15, L15, M15),1),     BIN2HEX(_xlfn.CONCAT(N15,O15,P15,Q15),1),     BIN2HEX(_xlfn.CONCAT(R15,S15,T15,U15),1),     BIN2HEX(_xlfn.CONCAT(V15,W15,X15,Y15),1),     BIN2HEX(_xlfn.CONCAT(Z15,AA15,AB15,AC15),1),     BIN2HEX(_xlfn.CONCAT(AD15,AE15,C15,D15),1),     BIN2HEX(_xlfn.CONCAT(E15,F15,G15,H15),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>408080E</v>
+      </c>
+      <c r="AJ15" s="33" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:43" ht="14.25" customHeight="1">
+    <row r="16" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B16" s="14"/>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C16" s="14">
         <v>0</v>
       </c>
@@ -2286,23 +2466,23 @@
         <v>0</v>
       </c>
       <c r="E16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="14">
         <v>0</v>
@@ -2322,8 +2502,8 @@
       <c r="P16" s="14">
         <v>0</v>
       </c>
-      <c r="Q16" s="14">
-        <v>0</v>
+      <c r="Q16" s="2">
+        <v>1</v>
       </c>
       <c r="R16" s="14">
         <v>0</v>
@@ -2338,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="14">
         <v>0</v>
@@ -2369,21 +2549,26 @@
       </c>
       <c r="AF16" s="4"/>
       <c r="AG16" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J16, K16, L16, M16),1),     BIN2HEX(_xlfn.CONCAT(N16,O16,P16,Q16),1),     BIN2HEX(_xlfn.CONCAT(R16,S16,T16,U16),1),     BIN2HEX(_xlfn.CONCAT(V16,W16,X16,Y16),1),     BIN2HEX(_xlfn.CONCAT(Z16,AA16,AB16,AC16),1),     BIN2HEX(_xlfn.CONCAT(AD16,AE16,C16,D16),1),     BIN2HEX(_xlfn.CONCAT(E16,F16,G16,H16),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>810800F</v>
+      </c>
+      <c r="AJ16" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="14.25" customHeight="1">
+    <row r="17" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B17" s="14"/>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="C17" s="14">
         <v>0</v>
       </c>
       <c r="D17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="14">
         <v>0</v>
@@ -2399,7 +2584,7 @@
       </c>
       <c r="I17" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J17" s="14">
         <v>0</v>
@@ -2429,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="S17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="14">
         <v>0</v>
@@ -2444,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="14">
         <v>0</v>
@@ -2469,16 +2654,21 @@
       </c>
       <c r="AF17" s="4"/>
       <c r="AG17" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J17, K17, L17, M17),1),     BIN2HEX(_xlfn.CONCAT(N17,O17,P17,Q17),1),     BIN2HEX(_xlfn.CONCAT(R17,S17,T17,U17),1),     BIN2HEX(_xlfn.CONCAT(V17,W17,X17,Y17),1),     BIN2HEX(_xlfn.CONCAT(Z17,AA17,AB17,AC17),1),     BIN2HEX(_xlfn.CONCAT(AD17,AE17,C17,D17),1),     BIN2HEX(_xlfn.CONCAT(E17,F17,G17,H17),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>0042010</v>
+      </c>
+      <c r="AJ17" s="33" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="14.25" customHeight="1">
+    <row r="18" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="B18" s="14"/>
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C18" s="14">
         <v>0</v>
       </c>
@@ -2520,7 +2710,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="14">
         <v>0</v>
@@ -2547,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="Y18" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18" s="14">
         <v>0</v>
@@ -2569,21 +2759,26 @@
       </c>
       <c r="AF18" s="4"/>
       <c r="AG18" s="6" t="str">
-        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(J18, K18, L18, M18),1),     BIN2HEX(_xlfn.CONCAT(N18,O18,P18,Q18),1),     BIN2HEX(_xlfn.CONCAT(R18,S18,T18,U18),1),     BIN2HEX(_xlfn.CONCAT(V18,W18,X18,Y18),1),     BIN2HEX(_xlfn.CONCAT(Z18,AA18,AB18,AC18),1),     BIN2HEX(_xlfn.CONCAT(AD18,AE18,C18,D18),1),     BIN2HEX(_xlfn.CONCAT(E18,F18,G18,H18),1) )</f>
-        <v>0000000</v>
+        <f t="shared" si="3"/>
+        <v>0201000</v>
+      </c>
+      <c r="AJ18" s="33" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="14.25" customHeight="1">
+    <row r="19" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="B19" s="14"/>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="C19" s="14">
         <v>0</v>
       </c>
       <c r="D19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="14">
         <v>0</v>
@@ -2592,20 +2787,20 @@
         <v>0</v>
       </c>
       <c r="G19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="14">
         <v>0</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J19" s="14">
         <v>0</v>
       </c>
       <c r="K19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="14">
         <v>0</v>
@@ -2626,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="R19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="14">
         <v>0</v>
@@ -2650,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="Z19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19" s="14">
         <v>0</v>
@@ -2670,20 +2865,25 @@
       <c r="AF19" s="4"/>
       <c r="AG19" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>4080812</v>
+      </c>
+      <c r="AJ19" s="33" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="14.25" customHeight="1">
+    <row r="20" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B20" s="14"/>
+      <c r="B20" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="C20" s="14">
         <v>0</v>
       </c>
       <c r="D20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="14">
         <v>0</v>
@@ -2692,17 +2892,17 @@
         <v>0</v>
       </c>
       <c r="G20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="14">
         <v>0</v>
@@ -2722,8 +2922,8 @@
       <c r="P20" s="14">
         <v>0</v>
       </c>
-      <c r="Q20" s="14">
-        <v>0</v>
+      <c r="Q20" s="2">
+        <v>1</v>
       </c>
       <c r="R20" s="14">
         <v>0</v>
@@ -2738,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="V20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="14">
         <v>0</v>
@@ -2770,26 +2970,31 @@
       <c r="AF20" s="4"/>
       <c r="AG20" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>8108013</v>
+      </c>
+      <c r="AJ20" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="14.25" customHeight="1">
+    <row r="21" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="B21" s="14"/>
+      <c r="B21" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C21" s="14">
         <v>0</v>
       </c>
       <c r="D21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="14">
         <v>0</v>
       </c>
       <c r="F21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="14">
         <v>0</v>
@@ -2799,7 +3004,7 @@
       </c>
       <c r="I21" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J21" s="14">
         <v>0</v>
@@ -2829,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="14">
         <v>0</v>
@@ -2844,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="14">
         <v>0</v>
@@ -2870,15 +3075,20 @@
       <c r="AF21" s="4"/>
       <c r="AG21" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0042014</v>
+      </c>
+      <c r="AJ21" s="33" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="14.25" customHeight="1">
+    <row r="22" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B22" s="14"/>
+      <c r="B22" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="C22" s="14">
         <v>0</v>
       </c>
@@ -2917,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="O22" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="14">
         <v>0</v>
@@ -2950,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="Z22" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22" s="14">
         <v>0</v>
@@ -2970,10 +3180,13 @@
       <c r="AF22" s="4"/>
       <c r="AG22" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0400800</v>
+      </c>
+      <c r="AJ22" s="33" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="14.25" customHeight="1">
+    <row r="23" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -3073,7 +3286,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="14.25" customHeight="1">
+    <row r="24" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -3173,7 +3386,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="14.25" customHeight="1">
+    <row r="25" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -3273,7 +3486,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="14.25" customHeight="1">
+    <row r="26" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -3373,7 +3586,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="14.25" customHeight="1">
+    <row r="27" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -3473,7 +3686,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="14.25" customHeight="1">
+    <row r="28" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -3573,7 +3786,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="14.25" customHeight="1">
+    <row r="29" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -3673,7 +3886,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="14.25" customHeight="1">
+    <row r="30" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -3773,7 +3986,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="14.25" customHeight="1">
+    <row r="31" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3873,7 +4086,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="14.25" customHeight="1">
+    <row r="32" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -3973,7 +4186,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" customHeight="1">
+    <row r="33" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -4073,9 +4286,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" customHeight="1">
+    <row r="34" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
-        <f t="shared" ref="A34:A41" si="3">A33+1</f>
+        <f t="shared" ref="A34:A41" si="4">A33+1</f>
         <v>32</v>
       </c>
       <c r="B34" s="2"/>
@@ -4098,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" ref="I34:I49" si="4">BIN2DEC(_xlfn.CONCAT(C34:H34))</f>
+        <f t="shared" ref="I34:I49" si="5">BIN2DEC(_xlfn.CONCAT(C34:H34))</f>
         <v>0</v>
       </c>
       <c r="J34" s="14">
@@ -4173,9 +4386,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" customHeight="1">
+    <row r="35" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="B35" s="2"/>
@@ -4198,7 +4411,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J35" s="14">
@@ -4273,9 +4486,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="16.05" customHeight="1">
+    <row r="36" spans="1:34" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="B36" s="2"/>
@@ -4298,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J36" s="14">
@@ -4373,9 +4586,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" customHeight="1">
+    <row r="37" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="B37" s="2"/>
@@ -4398,7 +4611,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J37" s="14">
@@ -4473,9 +4686,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" customHeight="1">
+    <row r="38" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="B38" s="2"/>
@@ -4498,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="15">
-        <f t="shared" ref="I38:I46" si="5">BIN2DEC(_xlfn.CONCAT(C38:H38))</f>
+        <f t="shared" ref="I38:I46" si="6">BIN2DEC(_xlfn.CONCAT(C38:H38))</f>
         <v>0</v>
       </c>
       <c r="J38" s="14">
@@ -4573,9 +4786,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" customHeight="1">
+    <row r="39" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="B39" s="2"/>
@@ -4598,7 +4811,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J39" s="14">
@@ -4676,9 +4889,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" customHeight="1">
+    <row r="40" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="B40" s="2"/>
@@ -4701,7 +4914,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J40" s="14">
@@ -4776,9 +4989,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" customHeight="1">
+    <row r="41" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="B41" s="2"/>
@@ -4801,7 +5014,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J41" s="14">
@@ -4876,9 +5089,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" customHeight="1">
+    <row r="42" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
-        <f t="shared" ref="A42:A65" si="6">A41+1</f>
+        <f t="shared" ref="A42:A65" si="7">A41+1</f>
         <v>40</v>
       </c>
       <c r="B42" s="2"/>
@@ -4901,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J42" s="14">
@@ -4976,7 +5189,7 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="14.25" customHeight="1">
+    <row r="43" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <f>A42+1</f>
         <v>41</v>
@@ -5001,7 +5214,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J43" s="14">
@@ -5076,9 +5289,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="14.25" customHeight="1">
+    <row r="44" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="B44" s="2"/>
@@ -5101,7 +5314,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J44" s="14">
@@ -5176,9 +5389,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="14.25" customHeight="1">
+    <row r="45" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="B45" s="2"/>
@@ -5201,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J45" s="14">
@@ -5276,9 +5489,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="14.25" customHeight="1">
+    <row r="46" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="B46" s="2"/>
@@ -5301,7 +5514,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J46" s="14">
@@ -5376,9 +5589,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="14.25" customHeight="1">
+    <row r="47" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="B47" s="2"/>
@@ -5401,7 +5614,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J47" s="14">
@@ -5476,9 +5689,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="48" spans="1:34" ht="14.25" customHeight="1">
+    <row r="48" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
       <c r="B48" s="2"/>
@@ -5501,7 +5714,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J48" s="14">
@@ -5576,9 +5789,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="49" spans="1:35" ht="14.25" customHeight="1">
+    <row r="49" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="B49" s="2"/>
@@ -5601,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J49" s="14">
@@ -5676,9 +5889,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="50" spans="1:35" ht="14.25" customHeight="1">
+    <row r="50" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="B50" s="2"/>
@@ -5701,7 +5914,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="15">
-        <f t="shared" ref="I50:I59" si="7">BIN2DEC(_xlfn.CONCAT(C50:H50))</f>
+        <f t="shared" ref="I50:I59" si="8">BIN2DEC(_xlfn.CONCAT(C50:H50))</f>
         <v>0</v>
       </c>
       <c r="J50" s="14">
@@ -5776,9 +5989,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="51" spans="1:35" ht="14.25" customHeight="1">
+    <row r="51" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="B51" s="2"/>
@@ -5801,7 +6014,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J51" s="14">
@@ -5876,9 +6089,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="52" spans="1:35" ht="14.25" customHeight="1">
+    <row r="52" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="B52" s="2"/>
@@ -5901,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J52" s="14">
@@ -5976,9 +6189,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="53" spans="1:35" ht="14.25" customHeight="1">
+    <row r="53" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>51</v>
       </c>
       <c r="B53" s="2"/>
@@ -6001,7 +6214,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J53" s="14">
@@ -6076,9 +6289,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="54" spans="1:35" ht="14.25" customHeight="1">
+    <row r="54" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>52</v>
       </c>
       <c r="B54" s="2"/>
@@ -6101,7 +6314,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J54" s="14">
@@ -6176,9 +6389,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="55" spans="1:35" ht="14.25" customHeight="1">
+    <row r="55" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
       <c r="B55" s="2"/>
@@ -6201,7 +6414,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J55" s="14">
@@ -6276,9 +6489,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="56" spans="1:35" ht="14.25" customHeight="1">
+    <row r="56" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
       <c r="B56" s="2"/>
@@ -6301,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J56" s="14">
@@ -6376,9 +6589,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="57" spans="1:35" ht="14.25" customHeight="1">
+    <row r="57" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
       <c r="B57" s="2"/>
@@ -6401,7 +6614,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J57" s="14">
@@ -6476,9 +6689,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="58" spans="1:35" ht="14.25" customHeight="1">
+    <row r="58" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="B58" s="2"/>
@@ -6501,7 +6714,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J58" s="14">
@@ -6576,9 +6789,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="59" spans="1:35" ht="14.25" customHeight="1">
+    <row r="59" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
       <c r="B59" s="2"/>
@@ -6601,7 +6814,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J59" s="14">
@@ -6676,9 +6889,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="60" spans="1:35" ht="14.25" customHeight="1">
+    <row r="60" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>58</v>
       </c>
       <c r="B60" s="2"/>
@@ -6701,7 +6914,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="15">
-        <f t="shared" ref="I60:I65" si="8">BIN2DEC(_xlfn.CONCAT(C60:H60))</f>
+        <f t="shared" ref="I60:I65" si="9">BIN2DEC(_xlfn.CONCAT(C60:H60))</f>
         <v>0</v>
       </c>
       <c r="J60" s="14">
@@ -6777,9 +6990,9 @@
       </c>
       <c r="AI60" s="1"/>
     </row>
-    <row r="61" spans="1:35" ht="14.25" customHeight="1">
+    <row r="61" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>59</v>
       </c>
       <c r="B61" s="2"/>
@@ -6802,7 +7015,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J61" s="14">
@@ -6877,9 +7090,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="62" spans="1:35" ht="14.25" customHeight="1">
+    <row r="62" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="B62" s="2"/>
@@ -6902,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J62" s="14">
@@ -6977,9 +7190,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="63" spans="1:35" ht="14.25" customHeight="1">
+    <row r="63" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
       <c r="B63" s="2"/>
@@ -7002,7 +7215,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J63" s="14">
@@ -7077,9 +7290,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="64" spans="1:35" ht="14.25" customHeight="1">
+    <row r="64" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>62</v>
       </c>
       <c r="B64" s="2"/>
@@ -7102,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J64" s="14">
@@ -7177,9 +7390,9 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="14.25" customHeight="1">
+    <row r="65" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>63</v>
       </c>
       <c r="B65" s="2"/>
@@ -7202,7 +7415,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J65" s="14">
@@ -7277,11 +7490,11 @@
         <v>0000000</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="14.25" customHeight="1"/>
-    <row r="67" spans="1:33" ht="14.25" customHeight="1">
+    <row r="66" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AF67" s="4"/>
     </row>
-    <row r="68" spans="1:33" ht="14.25" customHeight="1">
+    <row r="68" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="30" t="s">
         <v>22</v>
       </c>
@@ -7307,7 +7520,7 @@
       <c r="T68" s="26"/>
       <c r="U68" s="26"/>
     </row>
-    <row r="69" spans="1:33" ht="14.25" customHeight="1">
+    <row r="69" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="7" t="s">
         <v>24</v>
       </c>
@@ -7343,7 +7556,7 @@
       <c r="T69" s="26"/>
       <c r="U69" s="26"/>
     </row>
-    <row r="70" spans="1:33" ht="14.25" customHeight="1">
+    <row r="70" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="16"/>
       <c r="C70" s="25"/>
       <c r="D70" s="25"/>
@@ -7360,7 +7573,7 @@
       <c r="M70" s="20"/>
       <c r="N70" s="13"/>
       <c r="O70" s="9" t="str">
-        <f t="shared" ref="O70:O85" si="9">DEC2HEX(N70,2)</f>
+        <f t="shared" ref="O70:O85" si="10">DEC2HEX(N70,2)</f>
         <v>00</v>
       </c>
       <c r="Q70" s="26"/>
@@ -7369,7 +7582,7 @@
       <c r="T70" s="26"/>
       <c r="U70" s="26"/>
     </row>
-    <row r="71" spans="1:33" ht="14.25" customHeight="1">
+    <row r="71" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="16"/>
       <c r="C71" s="25"/>
       <c r="D71" s="25"/>
@@ -7386,7 +7599,7 @@
       <c r="M71" s="20"/>
       <c r="N71" s="13"/>
       <c r="O71" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q71" s="26"/>
@@ -7395,7 +7608,7 @@
       <c r="T71" s="26"/>
       <c r="U71" s="26"/>
     </row>
-    <row r="72" spans="1:33" ht="14.25" customHeight="1">
+    <row r="72" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="22"/>
       <c r="C72" s="25"/>
       <c r="D72" s="25"/>
@@ -7412,7 +7625,7 @@
       <c r="M72" s="20"/>
       <c r="N72" s="13"/>
       <c r="O72" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q72" s="26"/>
@@ -7421,7 +7634,7 @@
       <c r="T72" s="26"/>
       <c r="U72" s="26"/>
     </row>
-    <row r="73" spans="1:33" ht="14.25" customHeight="1">
+    <row r="73" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="23"/>
       <c r="C73" s="32"/>
       <c r="D73" s="32"/>
@@ -7431,14 +7644,14 @@
       <c r="H73" s="32"/>
       <c r="I73" s="24"/>
       <c r="J73" s="18" t="str">
-        <f t="shared" ref="J73" si="10">DEC2HEX(C73)</f>
+        <f t="shared" ref="J73" si="11">DEC2HEX(C73)</f>
         <v>0</v>
       </c>
       <c r="L73" s="19"/>
       <c r="M73" s="20"/>
       <c r="N73" s="13"/>
       <c r="O73" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q73" s="26"/>
@@ -7447,7 +7660,7 @@
       <c r="T73" s="26"/>
       <c r="U73" s="26"/>
     </row>
-    <row r="74" spans="1:33" ht="14.25" customHeight="1">
+    <row r="74" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" s="21"/>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
@@ -7459,16 +7672,16 @@
       <c r="M74" s="20"/>
       <c r="N74" s="13"/>
       <c r="O74" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="14.25" customHeight="1">
+    <row r="75" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L75" s="19"/>
       <c r="M75" s="20"/>
       <c r="N75" s="13"/>
       <c r="O75" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q75" s="27" t="s">
@@ -7479,12 +7692,12 @@
       <c r="T75" s="27"/>
       <c r="U75" s="27"/>
     </row>
-    <row r="76" spans="1:33" ht="14.25" customHeight="1">
+    <row r="76" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L76" s="19"/>
       <c r="M76" s="20"/>
       <c r="N76" s="13"/>
       <c r="O76" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q76" s="27"/>
@@ -7493,12 +7706,12 @@
       <c r="T76" s="27"/>
       <c r="U76" s="27"/>
     </row>
-    <row r="77" spans="1:33" ht="15" customHeight="1">
+    <row r="77" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L77" s="19"/>
       <c r="M77" s="20"/>
       <c r="N77" s="13"/>
       <c r="O77" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q77" s="27"/>
@@ -7507,12 +7720,12 @@
       <c r="T77" s="27"/>
       <c r="U77" s="27"/>
     </row>
-    <row r="78" spans="1:33" ht="14.25" customHeight="1">
+    <row r="78" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L78" s="10"/>
       <c r="M78" s="11"/>
       <c r="N78" s="13"/>
       <c r="O78" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q78" s="27"/>
@@ -7521,12 +7734,12 @@
       <c r="T78" s="27"/>
       <c r="U78" s="27"/>
     </row>
-    <row r="79" spans="1:33" ht="14.25" customHeight="1">
+    <row r="79" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L79" s="19"/>
       <c r="M79" s="20"/>
       <c r="N79" s="13"/>
       <c r="O79" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q79" s="27"/>
@@ -7535,12 +7748,12 @@
       <c r="T79" s="27"/>
       <c r="U79" s="27"/>
     </row>
-    <row r="80" spans="1:33" ht="14.25" customHeight="1">
+    <row r="80" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L80" s="10"/>
       <c r="M80" s="11"/>
       <c r="N80" s="13"/>
       <c r="O80" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="Q80" s="27"/>
@@ -7549,54 +7762,54 @@
       <c r="T80" s="27"/>
       <c r="U80" s="27"/>
     </row>
-    <row r="81" spans="12:15" ht="14.25" customHeight="1">
+    <row r="81" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L81" s="10"/>
       <c r="M81" s="11"/>
       <c r="N81" s="13"/>
       <c r="O81" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
-    <row r="82" spans="12:15" ht="14.25" customHeight="1">
+    <row r="82" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L82" s="10"/>
       <c r="M82" s="11"/>
       <c r="N82" s="13"/>
       <c r="O82" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
-    <row r="83" spans="12:15" ht="14.25" customHeight="1">
+    <row r="83" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L83" s="10"/>
       <c r="M83" s="11"/>
       <c r="N83" s="13"/>
       <c r="O83" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="12:15" ht="14.25" customHeight="1">
+    <row r="84" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L84" s="10"/>
       <c r="M84" s="11"/>
       <c r="O84" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
-    <row r="85" spans="12:15" ht="14.25" customHeight="1">
+    <row r="85" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L85" s="10"/>
       <c r="M85" s="11"/>
       <c r="O85" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
-    <row r="86" spans="12:15" ht="14.25" customHeight="1">
+    <row r="86" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L86" s="10"/>
       <c r="O86" s="12"/>
     </row>
-    <row r="87" spans="12:15" ht="14.25" customHeight="1">
+    <row r="87" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="L87" s="28" t="s">
         <v>31</v>
       </c>
@@ -7604,936 +7817,936 @@
       <c r="N87" s="28"/>
       <c r="O87" s="28"/>
     </row>
-    <row r="88" spans="12:15" ht="14.25" customHeight="1">
+    <row r="88" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="L88" s="28"/>
       <c r="M88" s="28"/>
       <c r="N88" s="28"/>
       <c r="O88" s="28"/>
     </row>
-    <row r="89" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="90" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="91" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="92" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="93" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="94" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="95" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="96" spans="12:15" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
-    <row r="1005" ht="14.25" customHeight="1"/>
-    <row r="1006" ht="14.25" customHeight="1"/>
-    <row r="1007" ht="14.25" customHeight="1"/>
-    <row r="1008" ht="14.25" customHeight="1"/>
-    <row r="1009" ht="14.25" customHeight="1"/>
-    <row r="1010" ht="14.25" customHeight="1"/>
-    <row r="1011" ht="14.25" customHeight="1"/>
-    <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="89" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" spans="12:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C71:H71"/>

</xml_diff>